<commit_message>
Mise a jour du 20/07/2025 a 23:04:43,82
</commit_message>
<xml_diff>
--- a/data/apports_investisseurs.xlsx
+++ b/data/apports_investisseurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dashboard Investissement\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CA738E-3B69-4B3A-818D-24B9A809D5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35137A2-C604-42FA-BAAF-9A9254A44245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{99A7773B-E842-47AD-9EDD-B9E3C5A4BAFD}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -132,19 +132,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,7 +481,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +500,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -513,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="4">
-        <v>10465</v>
+        <v>10365</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>

</xml_diff>